<commit_message>
Enhance model table validation and waste/resource handling
- Added ValidateModelTables.m for model file validation.
- Improved waste and resource cost table parsing, error handling, and type checking in cReadModelTable, cModelData, cWasteData, and related classes. -
- Updated cMessages with new error messages, - Improved cProductiveStructure and cModelTable for better key handling and display, and fixed minor bugs.
- Updated example models and added new chloralkaly example files.
</commit_message>
<xml_diff>
--- a/Examples/amoniaco/NH3_model.xlsx
+++ b/Examples/amoniaco/NH3_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ctorr\Documents\Proyectos\TaesLab\Examples\amoniaco\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7886D9-2A7C-4A02-858D-D05B9D1FAFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635A7943-CE57-4456-9A62-27A5A566ECC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2820" windowWidth="21600" windowHeight="11295" tabRatio="801" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="780" windowWidth="25740" windowHeight="14700" tabRatio="801" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PhysicalDiagram" sheetId="5" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="135">
   <si>
     <t>key</t>
   </si>
@@ -2042,16 +2042,17 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E1" sqref="E1:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.7109375" style="3" customWidth="1"/>
-    <col min="2" max="3" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="28" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="3"/>
+    <col min="2" max="2" width="14.140625" style="3" customWidth="1"/>
+    <col min="3" max="4" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="28" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2059,13 +2060,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>1</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>5</v>
@@ -2076,13 +2077,13 @@
         <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>45</v>
@@ -2093,13 +2094,13 @@
         <v>41</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>67</v>
@@ -2110,13 +2111,13 @@
         <v>42</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>63</v>
@@ -2127,13 +2128,13 @@
         <v>43</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>56</v>
@@ -2144,13 +2145,13 @@
         <v>44</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>58</v>
@@ -2161,13 +2162,13 @@
         <v>50</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>64</v>
@@ -2178,13 +2179,13 @@
         <v>51</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>65</v>
@@ -2195,13 +2196,13 @@
         <v>46</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>48</v>
@@ -2212,13 +2213,13 @@
         <v>47</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>98</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>49</v>
@@ -2228,14 +2229,14 @@
       <c r="A11" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>125</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>68</v>
@@ -2245,14 +2246,14 @@
       <c r="A12" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>66</v>
@@ -2262,14 +2263,14 @@
       <c r="A13" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="D13" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>55</v>
@@ -2279,14 +2280,14 @@
       <c r="A14" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>70</v>
@@ -2297,13 +2298,13 @@
         <v>52</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>71</v>
@@ -2314,13 +2315,13 @@
         <v>53</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>72</v>
@@ -2330,14 +2331,14 @@
       <c r="A17" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>73</v>
@@ -2348,13 +2349,13 @@
         <v>57</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>62</v>
@@ -2370,7 +2371,7 @@
           <x14:formula1>
             <xm:f>Validate!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D10</xm:sqref>
+          <xm:sqref>B2:B10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2943,7 +2944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0F86BC-BE05-47BA-8A3F-C728A67375A6}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
@@ -2985,21 +2986,21 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Hoja7"/>
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.85546875" style="3"/>
+    <col min="3" max="9" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3027,14 +3028,8 @@
       <c r="I1" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>114</v>
       </c>
@@ -3062,14 +3057,8 @@
       <c r="I2" s="10">
         <v>1.2844720496894411</v>
       </c>
-      <c r="J2" s="10">
-        <v>1.3888198757763976</v>
-      </c>
-      <c r="K2" s="10">
-        <v>1.7614906832298134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>115</v>
       </c>
@@ -3097,14 +3086,8 @@
       <c r="I3" s="10">
         <v>7.0149253731343286</v>
       </c>
-      <c r="J3" s="10">
-        <v>7.5848032564450483</v>
-      </c>
-      <c r="K3" s="10">
-        <v>9.6200814111261863</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>127</v>
       </c>
@@ -3132,14 +3115,8 @@
       <c r="I4" s="3">
         <v>0</v>
       </c>
-      <c r="J4" s="3">
-        <v>0</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>118</v>
       </c>
@@ -3167,14 +3144,8 @@
       <c r="I5" s="10">
         <v>1.034</v>
       </c>
-      <c r="J5" s="10">
-        <v>1.1180000000000001</v>
-      </c>
-      <c r="K5" s="10">
-        <v>1.4179999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>119</v>
       </c>
@@ -3202,14 +3173,8 @@
       <c r="I6" s="10">
         <v>1.034</v>
       </c>
-      <c r="J6" s="10">
-        <v>1.1180000000000001</v>
-      </c>
-      <c r="K6" s="10">
-        <v>1.4179999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
@@ -3220,10 +3185,8 @@
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-    </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -3232,12 +3195,10 @@
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
-      <c r="K10" s="12"/>
+      <c r="K10" s="8"/>
       <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
@@ -3246,12 +3207,10 @@
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
-      <c r="K11" s="12"/>
+      <c r="K11" s="8"/>
       <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -3260,12 +3219,10 @@
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
-      <c r="K12" s="12"/>
+      <c r="K12" s="8"/>
       <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -3276,10 +3233,8 @@
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -3290,10 +3245,8 @@
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
@@ -3304,10 +3257,8 @@
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -3316,10 +3267,8 @@
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -3328,10 +3277,8 @@
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -3340,10 +3287,8 @@
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -3352,10 +3297,8 @@
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
@@ -3364,10 +3307,8 @@
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -3376,10 +3317,8 @@
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -3388,8 +3327,6 @@
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>